<commit_message>
Do some stuff w/database and jobs page
</commit_message>
<xml_diff>
--- a/spreadsheets/jobSeeder.xlsx
+++ b/spreadsheets/jobSeeder.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pknipp/Dropbox/AppAcad/weeks/TaskRabbitClone/spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2773854D-DCBE-2C41-A1D2-F0DAFC8C0715}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68CF397F-11A8-5C4D-8E4C-0FCC92C245AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20560" xr2:uid="{B90A68FD-6178-6349-8A3B-C5FACB681F3A}"/>
   </bookViews>
@@ -403,7 +403,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E2" sqref="E2:E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -435,47 +435,47 @@
       </c>
       <c r="B2">
         <f ca="1">RANDBETWEEN(1,8)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="str">
         <f ca="1">_xlfn.CONCAT("2020-08-",RANDBETWEEN(10,31)," ",RANDBETWEEN(10,23),":",RANDBETWEEN(10,59),":",RANDBETWEEN(10,59))</f>
-        <v>2020-08-21 14:39:47</v>
+        <v>2020-08-31 16:26:41</v>
       </c>
       <c r="D2" s="1" t="str">
         <f ca="1">_xlfn.CONCAT("2020-0",RANDBETWEEN(7,9),"-",RANDBETWEEN(10,30),"")</f>
-        <v>2020-07-29</v>
+        <v>2020-08-16</v>
       </c>
       <c r="E2" t="str">
         <f ca="1">_xlfn.CONCAT("{userId:", A2, ",taskerId:", B2, ",jobDate:", D2, ",details:},")</f>
-        <v>{userId:1,taskerId:2,jobDate:2020-07-29,details:},</v>
+        <v>{userId:1,taskerId:5,jobDate:2020-08-16,details:},</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <f t="shared" ref="A3:A22" ca="1" si="0">RANDBETWEEN(1,3)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <f t="shared" ref="B3:B22" ca="1" si="1">RANDBETWEEN(1,8)</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1" t="str">
         <f t="shared" ref="C3:C22" ca="1" si="2">_xlfn.CONCAT("2020-08-",RANDBETWEEN(10,31)," ",RANDBETWEEN(10,23),":",RANDBETWEEN(10,59),":",RANDBETWEEN(10,59))</f>
-        <v>2020-08-31 10:40:50</v>
+        <v>2020-08-15 15:28:12</v>
       </c>
       <c r="D3" s="1" t="str">
         <f t="shared" ref="D3:D22" ca="1" si="3">_xlfn.CONCAT("2020-0",RANDBETWEEN(7,9),"-",RANDBETWEEN(10,30),"")</f>
-        <v>2020-09-10</v>
+        <v>2020-09-14</v>
       </c>
       <c r="E3" t="str">
         <f t="shared" ref="E3:E22" ca="1" si="4">_xlfn.CONCAT("{userId:", A3, ",taskerId:", B3, ",jobDate:", D3, ",details:},")</f>
-        <v>{userId:2,taskerId:2,jobDate:2020-09-10,details:},</v>
+        <v>{userId:3,taskerId:6,jobDate:2020-09-14,details:},</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="1"/>
@@ -483,15 +483,15 @@
       </c>
       <c r="C4" s="1" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>2020-08-10 16:42:46</v>
+        <v>2020-08-13 17:57:47</v>
       </c>
       <c r="D4" s="1" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>2020-08-19</v>
+        <v>2020-07-23</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>{userId:3,taskerId:8,jobDate:2020-08-19,details:},</v>
+        <v>{userId:1,taskerId:8,jobDate:2020-07-23,details:},</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -501,41 +501,41 @@
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C5" s="1" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>2020-08-13 20:52:25</v>
+        <v>2020-08-28 18:26:24</v>
       </c>
       <c r="D5" s="1" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>2020-08-10</v>
+        <v>2020-07-29</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>{userId:2,taskerId:6,jobDate:2020-08-10,details:},</v>
+        <v>{userId:2,taskerId:1,jobDate:2020-07-29,details:},</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" s="1" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>2020-08-17 21:53:35</v>
+        <v>2020-08-29 15:35:12</v>
       </c>
       <c r="D6" s="1" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>2020-07-27</v>
+        <v>2020-07-15</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>{userId:2,taskerId:7,jobDate:2020-07-27,details:},</v>
+        <v>{userId:1,taskerId:6,jobDate:2020-07-15,details:},</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -545,69 +545,69 @@
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C7" s="1" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>2020-08-29 15:24:26</v>
+        <v>2020-08-21 10:52:22</v>
       </c>
       <c r="D7" s="1" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>2020-08-16</v>
+        <v>2020-08-21</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>{userId:1,taskerId:7,jobDate:2020-08-16,details:},</v>
+        <v>{userId:1,taskerId:5,jobDate:2020-08-21,details:},</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C8" s="1" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>2020-08-28 10:21:17</v>
+        <v>2020-08-26 17:21:23</v>
       </c>
       <c r="D8" s="1" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>2020-07-21</v>
+        <v>2020-07-13</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>{userId:3,taskerId:2,jobDate:2020-07-21,details:},</v>
+        <v>{userId:1,taskerId:1,jobDate:2020-07-13,details:},</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C9" s="1" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>2020-08-30 12:26:44</v>
+        <v>2020-08-25 22:51:30</v>
       </c>
       <c r="D9" s="1" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>2020-09-13</v>
+        <v>2020-09-18</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>{userId:3,taskerId:5,jobDate:2020-09-13,details:},</v>
+        <v>{userId:2,taskerId:2,jobDate:2020-09-18,details:},</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="1"/>
@@ -615,81 +615,81 @@
       </c>
       <c r="C10" s="1" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>2020-08-20 11:55:46</v>
+        <v>2020-08-25 23:17:23</v>
       </c>
       <c r="D10" s="1" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>2020-08-10</v>
+        <v>2020-08-24</v>
       </c>
       <c r="E10" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>{userId:1,taskerId:2,jobDate:2020-08-10,details:},</v>
+        <v>{userId:3,taskerId:2,jobDate:2020-08-24,details:},</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C11" s="1" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>2020-08-29 21:36:45</v>
+        <v>2020-08-24 21:37:15</v>
       </c>
       <c r="D11" s="1" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>2020-08-21</v>
+        <v>2020-09-12</v>
       </c>
       <c r="E11" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>{userId:1,taskerId:6,jobDate:2020-08-21,details:},</v>
+        <v>{userId:3,taskerId:5,jobDate:2020-09-12,details:},</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C12" s="1" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>2020-08-27 20:56:50</v>
+        <v>2020-08-17 19:53:43</v>
       </c>
       <c r="D12" s="1" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>2020-08-11</v>
+        <v>2020-09-24</v>
       </c>
       <c r="E12" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>{userId:1,taskerId:6,jobDate:2020-08-11,details:},</v>
+        <v>{userId:2,taskerId:7,jobDate:2020-09-24,details:},</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C13" s="1" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>2020-08-14 10:37:41</v>
+        <v>2020-08-17 20:37:35</v>
       </c>
       <c r="D13" s="1" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>2020-07-16</v>
+        <v>2020-09-14</v>
       </c>
       <c r="E13" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>{userId:1,taskerId:2,jobDate:2020-07-16,details:},</v>
+        <v>{userId:2,taskerId:7,jobDate:2020-09-14,details:},</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -703,51 +703,51 @@
       </c>
       <c r="C14" s="1" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>2020-08-13 19:27:18</v>
+        <v>2020-08-16 22:51:37</v>
       </c>
       <c r="D14" s="1" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>2020-07-20</v>
+        <v>2020-08-23</v>
       </c>
       <c r="E14" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>{userId:2,taskerId:2,jobDate:2020-07-20,details:},</v>
+        <v>{userId:2,taskerId:2,jobDate:2020-08-23,details:},</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C15" s="1" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>2020-08-18 13:37:31</v>
+        <v>2020-08-17 11:21:29</v>
       </c>
       <c r="D15" s="1" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>2020-08-10</v>
+        <v>2020-09-23</v>
       </c>
       <c r="E15" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>{userId:1,taskerId:3,jobDate:2020-08-10,details:},</v>
+        <v>{userId:2,taskerId:8,jobDate:2020-09-23,details:},</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <f t="shared" ca="1" si="1"/>
         <v>3</v>
       </c>
-      <c r="B16">
-        <f t="shared" ca="1" si="1"/>
-        <v>8</v>
-      </c>
       <c r="C16" s="1" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>2020-08-11 19:11:11</v>
+        <v>2020-08-11 18:40:59</v>
       </c>
       <c r="D16" s="1" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -755,51 +755,51 @@
       </c>
       <c r="E16" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>{userId:3,taskerId:8,jobDate:2020-08-30,details:},</v>
+        <v>{userId:1,taskerId:3,jobDate:2020-08-30,details:},</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C17" s="1" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>2020-08-19 22:27:52</v>
+        <v>2020-08-10 14:56:59</v>
       </c>
       <c r="D17" s="1" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>2020-07-25</v>
+        <v>2020-09-29</v>
       </c>
       <c r="E17" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>{userId:2,taskerId:3,jobDate:2020-07-25,details:},</v>
+        <v>{userId:3,taskerId:1,jobDate:2020-09-29,details:},</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C18" s="1" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>2020-08-23 13:24:50</v>
+        <v>2020-08-18 16:49:17</v>
       </c>
       <c r="D18" s="1" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>2020-08-25</v>
+        <v>2020-09-18</v>
       </c>
       <c r="E18" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>{userId:2,taskerId:3,jobDate:2020-08-25,details:},</v>
+        <v>{userId:3,taskerId:8,jobDate:2020-09-18,details:},</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -809,85 +809,85 @@
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C19" s="1" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>2020-08-24 17:47:27</v>
+        <v>2020-08-17 23:58:15</v>
       </c>
       <c r="D19" s="1" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>2020-07-26</v>
+        <v>2020-07-17</v>
       </c>
       <c r="E19" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>{userId:1,taskerId:2,jobDate:2020-07-26,details:},</v>
+        <v>{userId:1,taskerId:6,jobDate:2020-07-17,details:},</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C20" s="1" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>2020-08-14 21:21:14</v>
+        <v>2020-08-13 10:21:49</v>
       </c>
       <c r="D20" s="1" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>2020-08-28</v>
+        <v>2020-07-29</v>
       </c>
       <c r="E20" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>{userId:1,taskerId:4,jobDate:2020-08-28,details:},</v>
+        <v>{userId:2,taskerId:6,jobDate:2020-07-29,details:},</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C21" s="1" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>2020-08-16 19:49:10</v>
+        <v>2020-08-30 20:14:25</v>
       </c>
       <c r="D21" s="1" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>2020-07-29</v>
+        <v>2020-09-25</v>
       </c>
       <c r="E21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>{userId:3,taskerId:2,jobDate:2020-07-29,details:},</v>
+        <v>{userId:2,taskerId:7,jobDate:2020-09-25,details:},</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B22">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C22" s="1" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>2020-08-27 19:19:11</v>
+        <v>2020-08-31 20:24:14</v>
       </c>
       <c r="D22" s="1" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>2020-07-28</v>
+        <v>2020-09-26</v>
       </c>
       <c r="E22" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>{userId:1,taskerId:6,jobDate:2020-07-28,details:},</v>
+        <v>{userId:3,taskerId:1,jobDate:2020-09-26,details:},</v>
       </c>
     </row>
   </sheetData>

</xml_diff>